<commit_message>
Manoj194 Pom pages added.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F31481-8148-4A21-851F-F9985499DF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CommonData" sheetId="1" r:id="rId1"/>
     <sheet name="Form" sheetId="3" r:id="rId2"/>
-    <sheet name="Module-name" sheetId="2" r:id="rId3"/>
+    <sheet name="AddingResturant" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="126">
   <si>
     <t>url</t>
   </si>
@@ -342,12 +343,69 @@
   </si>
   <si>
     <t>orderplacedmessage</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>PWD</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://rmgtestingserver/domain/Online_Food_Ordering_System/admin</t>
+  </si>
+  <si>
+    <t>Dropdownvalue</t>
+  </si>
+  <si>
+    <t>10am</t>
+  </si>
+  <si>
+    <t>Dropdowntext</t>
+  </si>
+  <si>
+    <t>Mon-Fri</t>
+  </si>
+  <si>
+    <t>Dropdownvalue2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indian </t>
+  </si>
+  <si>
+    <t>Dropdowntext2</t>
+  </si>
+  <si>
+    <t>6pm</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Resturant_name</t>
+  </si>
+  <si>
+    <t>Navarang resturant</t>
+  </si>
+  <si>
+    <t>mob_no</t>
+  </si>
+  <si>
+    <t>manuvirat775@gmail.com</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>www.https.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,7 +758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1054,10 +1112,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="http://rmgtestingserver/domain/Online_Food_Ordering_System/dishes.php?res_id=2"/>
-    <hyperlink ref="B19" r:id="rId2"/>
-    <hyperlink ref="C19" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId1" display="http://rmgtestingserver/domain/Online_Food_Ordering_System/dishes.php?res_id=2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -1065,10 +1123,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1208,9 +1266,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1218,13 +1276,122 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="68" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9902990508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{A156FB22-8659-43D4-9AD0-F81E7C3D277A}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{A0279573-D85D-4362-88B4-B6D4950815E2}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{3BA2BE82-15F4-4A4A-BDE9-3A45D6DCD622}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>